<commit_message>
added home module with data provider, login module with data provider and excel for data provider
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="97">
   <si>
     <t>username</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>Creating Linked LIst</t>
+  </si>
+  <si>
+    <t>Registration</t>
   </si>
 </sst>
 </file>
@@ -804,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,6 +1158,11 @@
     <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Tree Module with Try editor and excel data for dataprovider
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -809,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>